<commit_message>
Add level-based supervision schedule generation
- Support for grade levels (المستوى الأول، المستوى الثاني, etc.)
- Users can select level and generate separate schedules
- Updated sample data with level column
- Enhanced UI with level selection cards
- Export includes level name in filename and PDF
- Backward compatible with grade-based systems
</commit_message>
<xml_diff>
--- a/data_samples/exams.xlsx
+++ b/data_samples/exams.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>grade</t>
+          <t>level</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>الثالث</t>
+          <t>المستوى الأول</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>الثالث</t>
+          <t>المستوى الأول</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -548,22 +548,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>العلوم</t>
+          <t>الرياضيات</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>الرابع</t>
+          <t>المستوى الثاني</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>الثالث</t>
+          <t>المستوى الأول</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>الرابع</t>
+          <t>المستوى الثاني</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -653,22 +653,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>التربية الإسلامية</t>
+          <t>العلوم</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>الخامس</t>
+          <t>المستوى الثاني</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -703,12 +703,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>الرابع</t>
+          <t>المستوى الأول</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>الخامس</t>
+          <t>المستوى الثاني</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>الثالث</t>
+          <t>المستوى الأول</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>الرابع</t>
+          <t>المستوى الثاني</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">

</xml_diff>